<commit_message>
control cambio y estado avance proyecto
</commit_message>
<xml_diff>
--- a/Universidad-20230227T013253Z-001/Universidad/U 2023-1/gestion Proyectos ti/Control Cambio.xlsx
+++ b/Universidad-20230227T013253Z-001/Universidad/U 2023-1/gestion Proyectos ti/Control Cambio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlejandroGalleguillo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexis\Documents\GitHub\Universidad\Universidad-20230227T013253Z-001\Universidad\U 2023-1\gestion Proyectos ti\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA312FA7-02C1-475A-B2D4-EFF2169CAEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato Gestión del Cambio" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>Cargo</t>
   </si>
@@ -135,9 +136,6 @@
     <t>Interesados</t>
   </si>
   <si>
-    <t>Código Proyecto:</t>
-  </si>
-  <si>
     <t>Diseño</t>
   </si>
   <si>
@@ -148,13 +146,82 @@
   </si>
   <si>
     <t>Equipo</t>
+  </si>
+  <si>
+    <t>Brayan Alexis Maldonado Carraco</t>
+  </si>
+  <si>
+    <t>Jefe de proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>sector de cursos</t>
+  </si>
+  <si>
+    <t>Se ha buscado un profesional capacitado en el area de la docencia para mejorar la calidad de los cursos, lo cual ha implicado un retraso debido a la busqueda del mismo.</t>
+  </si>
+  <si>
+    <t>Alcance: Los cursos seran de mejor calidad.2)Costo:El costo aumenta ya que hay que pagarle al profesional capacitado.3)No se pueden agregar los cursos debido a que el profesional debe prepararlos con tiempo.</t>
+  </si>
+  <si>
+    <t>Proceso de selección del nuevo docente</t>
+  </si>
+  <si>
+    <t>Proceso de eliminacion del antiguo docente</t>
+  </si>
+  <si>
+    <t>Proceso de contratacion del nuevo docente</t>
+  </si>
+  <si>
+    <t>Prueba tecnica del nuevo docente</t>
+  </si>
+  <si>
+    <t>1) No encontrar un docente en la fecha estimada del cambio.                                 2) Que el docente no cumpla con las espectativas.</t>
+  </si>
+  <si>
+    <t>Personas afectadas: Proyecto en general y area de RR.HH</t>
+  </si>
+  <si>
+    <t>RR.HH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Delmonte(RR.HH)</t>
+  </si>
+  <si>
+    <t>Código Proyecto: ADM-R-P-2023-002</t>
+  </si>
+  <si>
+    <t>completado</t>
+  </si>
+  <si>
+    <t>pendiente</t>
+  </si>
+  <si>
+    <t>Juan Vélez Torres</t>
+  </si>
+  <si>
+    <t>Subgerente de Administración</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Carlos Delmonte</t>
+  </si>
+  <si>
+    <t>Jefe recursos humanos</t>
+  </si>
+  <si>
+    <t>Gerencia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,13 +266,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="8"/>
-      <name val="Humanst521 BT"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Humanst521 BT"/>
@@ -221,6 +281,23 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Humanst521 BT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Humanst521 BT"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Humanst521 BT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="8"/>
       <name val="Humanst521 BT"/>
       <family val="2"/>
     </font>
@@ -591,13 +668,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -609,251 +686,261 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -866,6 +953,135 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>35170</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>24348</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>398585</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>418465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5A75A7-6210-ECD8-3935-8265B7331F32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8475785" y="6214133"/>
+          <a:ext cx="363415" cy="394117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>87923</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>70339</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604877</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>409461</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E8DD59-3C57-C39D-24F7-98E3ADA3FEAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8528538" y="6881447"/>
+          <a:ext cx="516954" cy="339122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1130,1230 +1346,1112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IT29"/>
+  <dimension ref="A1:IR29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="83" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="83" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="31.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="31.33203125" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="8" style="11" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="11" style="10" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7" style="10" customWidth="1"/>
-    <col min="7" max="7" width="11" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="10" style="10" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="24" style="10" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="31.28515625" style="11"/>
+    <col min="1" max="1" width="14.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7" style="8" customWidth="1"/>
+    <col min="7" max="7" width="11" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="10" style="8" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="24" style="8" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="31.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:254" s="9" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A1" s="52"/>
-      <c r="B1" s="46" t="s">
+    <row r="1" spans="1:252" ht="16.5" customHeight="1">
+      <c r="A1" s="11"/>
+      <c r="B1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="8"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="88"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
       <c r="AB1" s="3"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="3"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
       <c r="AR1" s="3"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
       <c r="AZ1" s="3"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
       <c r="BC1" s="1"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
       <c r="BF1" s="1"/>
       <c r="BG1" s="1"/>
       <c r="BH1" s="3"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
       <c r="BK1" s="1"/>
       <c r="BL1" s="1"/>
       <c r="BM1" s="1"/>
       <c r="BN1" s="1"/>
       <c r="BO1" s="1"/>
       <c r="BP1" s="3"/>
-      <c r="BQ1" s="2"/>
-      <c r="BR1" s="2"/>
       <c r="BS1" s="1"/>
       <c r="BT1" s="1"/>
       <c r="BU1" s="1"/>
       <c r="BV1" s="1"/>
       <c r="BW1" s="1"/>
       <c r="BX1" s="3"/>
-      <c r="BY1" s="2"/>
-      <c r="BZ1" s="2"/>
       <c r="CA1" s="1"/>
       <c r="CB1" s="1"/>
       <c r="CC1" s="1"/>
       <c r="CD1" s="1"/>
       <c r="CE1" s="1"/>
       <c r="CF1" s="3"/>
-      <c r="CG1" s="2"/>
-      <c r="CH1" s="2"/>
       <c r="CI1" s="1"/>
       <c r="CJ1" s="1"/>
       <c r="CK1" s="1"/>
       <c r="CL1" s="1"/>
       <c r="CM1" s="1"/>
       <c r="CN1" s="3"/>
-      <c r="CO1" s="2"/>
-      <c r="CP1" s="2"/>
       <c r="CQ1" s="1"/>
       <c r="CR1" s="1"/>
       <c r="CS1" s="1"/>
       <c r="CT1" s="1"/>
       <c r="CU1" s="1"/>
       <c r="CV1" s="3"/>
-      <c r="CW1" s="2"/>
-      <c r="CX1" s="2"/>
       <c r="CY1" s="1"/>
       <c r="CZ1" s="1"/>
       <c r="DA1" s="1"/>
       <c r="DB1" s="1"/>
       <c r="DC1" s="1"/>
       <c r="DD1" s="3"/>
-      <c r="DE1" s="2"/>
-      <c r="DF1" s="2"/>
       <c r="DG1" s="1"/>
       <c r="DH1" s="1"/>
       <c r="DI1" s="1"/>
       <c r="DJ1" s="1"/>
       <c r="DK1" s="1"/>
       <c r="DL1" s="3"/>
-      <c r="DM1" s="2"/>
-      <c r="DN1" s="2"/>
       <c r="DO1" s="1"/>
       <c r="DP1" s="1"/>
       <c r="DQ1" s="1"/>
       <c r="DR1" s="1"/>
       <c r="DS1" s="1"/>
       <c r="DT1" s="3"/>
-      <c r="DU1" s="2"/>
-      <c r="DV1" s="2"/>
       <c r="DW1" s="1"/>
       <c r="DX1" s="1"/>
       <c r="DY1" s="1"/>
       <c r="DZ1" s="1"/>
       <c r="EA1" s="1"/>
       <c r="EB1" s="3"/>
-      <c r="EC1" s="2"/>
-      <c r="ED1" s="2"/>
       <c r="EE1" s="1"/>
       <c r="EF1" s="1"/>
       <c r="EG1" s="1"/>
       <c r="EH1" s="1"/>
       <c r="EI1" s="1"/>
       <c r="EJ1" s="3"/>
-      <c r="EK1" s="2"/>
-      <c r="EL1" s="2"/>
       <c r="EM1" s="1"/>
       <c r="EN1" s="1"/>
       <c r="EO1" s="1"/>
       <c r="EP1" s="1"/>
       <c r="EQ1" s="1"/>
       <c r="ER1" s="3"/>
-      <c r="ES1" s="2"/>
-      <c r="ET1" s="2"/>
       <c r="EU1" s="1"/>
       <c r="EV1" s="1"/>
       <c r="EW1" s="1"/>
       <c r="EX1" s="1"/>
       <c r="EY1" s="1"/>
       <c r="EZ1" s="3"/>
-      <c r="FA1" s="2"/>
-      <c r="FB1" s="2"/>
       <c r="FC1" s="1"/>
       <c r="FD1" s="1"/>
       <c r="FE1" s="1"/>
       <c r="FF1" s="1"/>
       <c r="FG1" s="1"/>
       <c r="FH1" s="3"/>
-      <c r="FI1" s="2"/>
-      <c r="FJ1" s="2"/>
       <c r="FK1" s="1"/>
       <c r="FL1" s="1"/>
       <c r="FM1" s="1"/>
       <c r="FN1" s="1"/>
       <c r="FO1" s="1"/>
       <c r="FP1" s="3"/>
-      <c r="FQ1" s="2"/>
-      <c r="FR1" s="2"/>
       <c r="FS1" s="1"/>
       <c r="FT1" s="1"/>
       <c r="FU1" s="1"/>
       <c r="FV1" s="1"/>
       <c r="FW1" s="1"/>
       <c r="FX1" s="3"/>
-      <c r="FY1" s="2"/>
-      <c r="FZ1" s="2"/>
       <c r="GA1" s="1"/>
       <c r="GB1" s="1"/>
       <c r="GC1" s="1"/>
       <c r="GD1" s="1"/>
       <c r="GE1" s="1"/>
       <c r="GF1" s="3"/>
-      <c r="GG1" s="2"/>
-      <c r="GH1" s="2"/>
       <c r="GI1" s="1"/>
       <c r="GJ1" s="1"/>
       <c r="GK1" s="1"/>
       <c r="GL1" s="1"/>
       <c r="GM1" s="1"/>
       <c r="GN1" s="3"/>
-      <c r="GO1" s="2"/>
-      <c r="GP1" s="2"/>
       <c r="GQ1" s="1"/>
       <c r="GR1" s="1"/>
       <c r="GS1" s="1"/>
       <c r="GT1" s="1"/>
       <c r="GU1" s="1"/>
       <c r="GV1" s="3"/>
-      <c r="GW1" s="2"/>
-      <c r="GX1" s="2"/>
       <c r="GY1" s="1"/>
       <c r="GZ1" s="1"/>
       <c r="HA1" s="1"/>
       <c r="HB1" s="1"/>
       <c r="HC1" s="1"/>
       <c r="HD1" s="3"/>
-      <c r="HE1" s="2"/>
-      <c r="HF1" s="2"/>
       <c r="HG1" s="1"/>
       <c r="HH1" s="1"/>
       <c r="HI1" s="1"/>
       <c r="HJ1" s="1"/>
       <c r="HK1" s="1"/>
       <c r="HL1" s="3"/>
-      <c r="HM1" s="2"/>
-      <c r="HN1" s="2"/>
       <c r="HO1" s="1"/>
       <c r="HP1" s="1"/>
       <c r="HQ1" s="1"/>
       <c r="HR1" s="1"/>
       <c r="HS1" s="1"/>
       <c r="HT1" s="3"/>
-      <c r="HU1" s="2"/>
-      <c r="HV1" s="2"/>
       <c r="HW1" s="1"/>
       <c r="HX1" s="1"/>
       <c r="HY1" s="1"/>
       <c r="HZ1" s="1"/>
       <c r="IA1" s="1"/>
       <c r="IB1" s="3"/>
-      <c r="IC1" s="2"/>
-      <c r="ID1" s="2"/>
       <c r="IE1" s="1"/>
       <c r="IF1" s="1"/>
       <c r="IG1" s="1"/>
       <c r="IH1" s="1"/>
       <c r="II1" s="1"/>
       <c r="IJ1" s="3"/>
-      <c r="IK1" s="2"/>
-      <c r="IL1" s="2"/>
       <c r="IM1" s="1"/>
       <c r="IN1" s="1"/>
       <c r="IO1" s="1"/>
       <c r="IP1" s="1"/>
       <c r="IQ1" s="1"/>
       <c r="IR1" s="3"/>
-      <c r="IS1" s="2"/>
-      <c r="IT1" s="2"/>
-    </row>
-    <row r="2" spans="1:254" s="9" customFormat="1" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A2" s="53"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="45"/>
+    </row>
+    <row r="2" spans="1:252" ht="12.75" customHeight="1" thickBot="1">
+      <c r="A2" s="12"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="90"/>
       <c r="L2" s="3"/>
       <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="3"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="3"/>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="2"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
       <c r="AQ2" s="1"/>
       <c r="AR2" s="3"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
       <c r="AZ2" s="3"/>
-      <c r="BA2" s="2"/>
-      <c r="BB2" s="2"/>
       <c r="BC2" s="1"/>
       <c r="BD2" s="1"/>
       <c r="BE2" s="1"/>
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
       <c r="BH2" s="3"/>
-      <c r="BI2" s="2"/>
-      <c r="BJ2" s="2"/>
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
       <c r="BN2" s="1"/>
       <c r="BO2" s="1"/>
       <c r="BP2" s="3"/>
-      <c r="BQ2" s="2"/>
-      <c r="BR2" s="2"/>
       <c r="BS2" s="1"/>
       <c r="BT2" s="1"/>
       <c r="BU2" s="1"/>
       <c r="BV2" s="1"/>
       <c r="BW2" s="1"/>
       <c r="BX2" s="3"/>
-      <c r="BY2" s="2"/>
-      <c r="BZ2" s="2"/>
       <c r="CA2" s="1"/>
       <c r="CB2" s="1"/>
       <c r="CC2" s="1"/>
       <c r="CD2" s="1"/>
       <c r="CE2" s="1"/>
       <c r="CF2" s="3"/>
-      <c r="CG2" s="2"/>
-      <c r="CH2" s="2"/>
       <c r="CI2" s="1"/>
       <c r="CJ2" s="1"/>
       <c r="CK2" s="1"/>
       <c r="CL2" s="1"/>
       <c r="CM2" s="1"/>
       <c r="CN2" s="3"/>
-      <c r="CO2" s="2"/>
-      <c r="CP2" s="2"/>
       <c r="CQ2" s="1"/>
       <c r="CR2" s="1"/>
       <c r="CS2" s="1"/>
       <c r="CT2" s="1"/>
       <c r="CU2" s="1"/>
       <c r="CV2" s="3"/>
-      <c r="CW2" s="2"/>
-      <c r="CX2" s="2"/>
       <c r="CY2" s="1"/>
       <c r="CZ2" s="1"/>
       <c r="DA2" s="1"/>
       <c r="DB2" s="1"/>
       <c r="DC2" s="1"/>
       <c r="DD2" s="3"/>
-      <c r="DE2" s="2"/>
-      <c r="DF2" s="2"/>
       <c r="DG2" s="1"/>
       <c r="DH2" s="1"/>
       <c r="DI2" s="1"/>
       <c r="DJ2" s="1"/>
       <c r="DK2" s="1"/>
       <c r="DL2" s="3"/>
-      <c r="DM2" s="2"/>
-      <c r="DN2" s="2"/>
       <c r="DO2" s="1"/>
       <c r="DP2" s="1"/>
       <c r="DQ2" s="1"/>
       <c r="DR2" s="1"/>
       <c r="DS2" s="1"/>
       <c r="DT2" s="3"/>
-      <c r="DU2" s="2"/>
-      <c r="DV2" s="2"/>
       <c r="DW2" s="1"/>
       <c r="DX2" s="1"/>
       <c r="DY2" s="1"/>
       <c r="DZ2" s="1"/>
       <c r="EA2" s="1"/>
       <c r="EB2" s="3"/>
-      <c r="EC2" s="2"/>
-      <c r="ED2" s="2"/>
       <c r="EE2" s="1"/>
       <c r="EF2" s="1"/>
       <c r="EG2" s="1"/>
       <c r="EH2" s="1"/>
       <c r="EI2" s="1"/>
       <c r="EJ2" s="3"/>
-      <c r="EK2" s="2"/>
-      <c r="EL2" s="2"/>
       <c r="EM2" s="1"/>
       <c r="EN2" s="1"/>
       <c r="EO2" s="1"/>
       <c r="EP2" s="1"/>
       <c r="EQ2" s="1"/>
       <c r="ER2" s="3"/>
-      <c r="ES2" s="2"/>
-      <c r="ET2" s="2"/>
       <c r="EU2" s="1"/>
       <c r="EV2" s="1"/>
       <c r="EW2" s="1"/>
       <c r="EX2" s="1"/>
       <c r="EY2" s="1"/>
       <c r="EZ2" s="3"/>
-      <c r="FA2" s="2"/>
-      <c r="FB2" s="2"/>
       <c r="FC2" s="1"/>
       <c r="FD2" s="1"/>
       <c r="FE2" s="1"/>
       <c r="FF2" s="1"/>
       <c r="FG2" s="1"/>
       <c r="FH2" s="3"/>
-      <c r="FI2" s="2"/>
-      <c r="FJ2" s="2"/>
       <c r="FK2" s="1"/>
       <c r="FL2" s="1"/>
       <c r="FM2" s="1"/>
       <c r="FN2" s="1"/>
       <c r="FO2" s="1"/>
       <c r="FP2" s="3"/>
-      <c r="FQ2" s="2"/>
-      <c r="FR2" s="2"/>
       <c r="FS2" s="1"/>
       <c r="FT2" s="1"/>
       <c r="FU2" s="1"/>
       <c r="FV2" s="1"/>
       <c r="FW2" s="1"/>
       <c r="FX2" s="3"/>
-      <c r="FY2" s="2"/>
-      <c r="FZ2" s="2"/>
       <c r="GA2" s="1"/>
       <c r="GB2" s="1"/>
       <c r="GC2" s="1"/>
       <c r="GD2" s="1"/>
       <c r="GE2" s="1"/>
       <c r="GF2" s="3"/>
-      <c r="GG2" s="2"/>
-      <c r="GH2" s="2"/>
       <c r="GI2" s="1"/>
       <c r="GJ2" s="1"/>
       <c r="GK2" s="1"/>
       <c r="GL2" s="1"/>
       <c r="GM2" s="1"/>
       <c r="GN2" s="3"/>
-      <c r="GO2" s="2"/>
-      <c r="GP2" s="2"/>
       <c r="GQ2" s="1"/>
       <c r="GR2" s="1"/>
       <c r="GS2" s="1"/>
       <c r="GT2" s="1"/>
       <c r="GU2" s="1"/>
       <c r="GV2" s="3"/>
-      <c r="GW2" s="2"/>
-      <c r="GX2" s="2"/>
       <c r="GY2" s="1"/>
       <c r="GZ2" s="1"/>
       <c r="HA2" s="1"/>
       <c r="HB2" s="1"/>
       <c r="HC2" s="1"/>
       <c r="HD2" s="3"/>
-      <c r="HE2" s="2"/>
-      <c r="HF2" s="2"/>
       <c r="HG2" s="1"/>
       <c r="HH2" s="1"/>
       <c r="HI2" s="1"/>
       <c r="HJ2" s="1"/>
       <c r="HK2" s="1"/>
       <c r="HL2" s="3"/>
-      <c r="HM2" s="2"/>
-      <c r="HN2" s="2"/>
       <c r="HO2" s="1"/>
       <c r="HP2" s="1"/>
       <c r="HQ2" s="1"/>
       <c r="HR2" s="1"/>
       <c r="HS2" s="1"/>
       <c r="HT2" s="3"/>
-      <c r="HU2" s="2"/>
-      <c r="HV2" s="2"/>
       <c r="HW2" s="1"/>
       <c r="HX2" s="1"/>
       <c r="HY2" s="1"/>
       <c r="HZ2" s="1"/>
       <c r="IA2" s="1"/>
       <c r="IB2" s="3"/>
-      <c r="IC2" s="2"/>
-      <c r="ID2" s="2"/>
       <c r="IE2" s="1"/>
       <c r="IF2" s="1"/>
       <c r="IG2" s="1"/>
       <c r="IH2" s="1"/>
       <c r="II2" s="1"/>
       <c r="IJ2" s="3"/>
-      <c r="IK2" s="2"/>
-      <c r="IL2" s="2"/>
       <c r="IM2" s="1"/>
       <c r="IN2" s="1"/>
       <c r="IO2" s="1"/>
       <c r="IP2" s="1"/>
       <c r="IQ2" s="1"/>
       <c r="IR2" s="3"/>
-      <c r="IS2" s="2"/>
-      <c r="IT2" s="2"/>
-    </row>
-    <row r="3" spans="1:254" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="31" t="s">
+    </row>
+    <row r="3" spans="1:252" ht="30" customHeight="1">
+      <c r="A3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="51"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="3"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="3"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="3"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="3"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="3"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
       <c r="BC3" s="1"/>
       <c r="BD3" s="1"/>
       <c r="BE3" s="1"/>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
       <c r="BH3" s="3"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
       <c r="BK3" s="1"/>
       <c r="BL3" s="1"/>
       <c r="BM3" s="1"/>
       <c r="BN3" s="1"/>
       <c r="BO3" s="1"/>
       <c r="BP3" s="3"/>
-      <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
       <c r="BS3" s="1"/>
       <c r="BT3" s="1"/>
       <c r="BU3" s="1"/>
       <c r="BV3" s="1"/>
       <c r="BW3" s="1"/>
       <c r="BX3" s="3"/>
-      <c r="BY3" s="2"/>
-      <c r="BZ3" s="2"/>
       <c r="CA3" s="1"/>
       <c r="CB3" s="1"/>
       <c r="CC3" s="1"/>
       <c r="CD3" s="1"/>
       <c r="CE3" s="1"/>
       <c r="CF3" s="3"/>
-      <c r="CG3" s="2"/>
-      <c r="CH3" s="2"/>
       <c r="CI3" s="1"/>
       <c r="CJ3" s="1"/>
       <c r="CK3" s="1"/>
       <c r="CL3" s="1"/>
       <c r="CM3" s="1"/>
       <c r="CN3" s="3"/>
-      <c r="CO3" s="2"/>
-      <c r="CP3" s="2"/>
       <c r="CQ3" s="1"/>
       <c r="CR3" s="1"/>
       <c r="CS3" s="1"/>
       <c r="CT3" s="1"/>
       <c r="CU3" s="1"/>
       <c r="CV3" s="3"/>
-      <c r="CW3" s="2"/>
-      <c r="CX3" s="2"/>
       <c r="CY3" s="1"/>
       <c r="CZ3" s="1"/>
       <c r="DA3" s="1"/>
       <c r="DB3" s="1"/>
       <c r="DC3" s="1"/>
       <c r="DD3" s="3"/>
-      <c r="DE3" s="2"/>
-      <c r="DF3" s="2"/>
       <c r="DG3" s="1"/>
       <c r="DH3" s="1"/>
       <c r="DI3" s="1"/>
       <c r="DJ3" s="1"/>
       <c r="DK3" s="1"/>
       <c r="DL3" s="3"/>
-      <c r="DM3" s="2"/>
-      <c r="DN3" s="2"/>
       <c r="DO3" s="1"/>
       <c r="DP3" s="1"/>
       <c r="DQ3" s="1"/>
       <c r="DR3" s="1"/>
       <c r="DS3" s="1"/>
       <c r="DT3" s="3"/>
-      <c r="DU3" s="2"/>
-      <c r="DV3" s="2"/>
       <c r="DW3" s="1"/>
       <c r="DX3" s="1"/>
       <c r="DY3" s="1"/>
       <c r="DZ3" s="1"/>
       <c r="EA3" s="1"/>
       <c r="EB3" s="3"/>
-      <c r="EC3" s="2"/>
-      <c r="ED3" s="2"/>
       <c r="EE3" s="1"/>
       <c r="EF3" s="1"/>
       <c r="EG3" s="1"/>
       <c r="EH3" s="1"/>
       <c r="EI3" s="1"/>
       <c r="EJ3" s="3"/>
-      <c r="EK3" s="2"/>
-      <c r="EL3" s="2"/>
       <c r="EM3" s="1"/>
       <c r="EN3" s="1"/>
       <c r="EO3" s="1"/>
       <c r="EP3" s="1"/>
       <c r="EQ3" s="1"/>
       <c r="ER3" s="3"/>
-      <c r="ES3" s="2"/>
-      <c r="ET3" s="2"/>
       <c r="EU3" s="1"/>
       <c r="EV3" s="1"/>
       <c r="EW3" s="1"/>
       <c r="EX3" s="1"/>
       <c r="EY3" s="1"/>
       <c r="EZ3" s="3"/>
-      <c r="FA3" s="2"/>
-      <c r="FB3" s="2"/>
       <c r="FC3" s="1"/>
       <c r="FD3" s="1"/>
       <c r="FE3" s="1"/>
       <c r="FF3" s="1"/>
       <c r="FG3" s="1"/>
       <c r="FH3" s="3"/>
-      <c r="FI3" s="2"/>
-      <c r="FJ3" s="2"/>
       <c r="FK3" s="1"/>
       <c r="FL3" s="1"/>
       <c r="FM3" s="1"/>
       <c r="FN3" s="1"/>
       <c r="FO3" s="1"/>
       <c r="FP3" s="3"/>
-      <c r="FQ3" s="2"/>
-      <c r="FR3" s="2"/>
       <c r="FS3" s="1"/>
       <c r="FT3" s="1"/>
       <c r="FU3" s="1"/>
       <c r="FV3" s="1"/>
       <c r="FW3" s="1"/>
       <c r="FX3" s="3"/>
-      <c r="FY3" s="2"/>
-      <c r="FZ3" s="2"/>
       <c r="GA3" s="1"/>
       <c r="GB3" s="1"/>
       <c r="GC3" s="1"/>
       <c r="GD3" s="1"/>
       <c r="GE3" s="1"/>
       <c r="GF3" s="3"/>
-      <c r="GG3" s="2"/>
-      <c r="GH3" s="2"/>
       <c r="GI3" s="1"/>
       <c r="GJ3" s="1"/>
       <c r="GK3" s="1"/>
       <c r="GL3" s="1"/>
       <c r="GM3" s="1"/>
       <c r="GN3" s="3"/>
-      <c r="GO3" s="2"/>
-      <c r="GP3" s="2"/>
       <c r="GQ3" s="1"/>
       <c r="GR3" s="1"/>
       <c r="GS3" s="1"/>
       <c r="GT3" s="1"/>
       <c r="GU3" s="1"/>
       <c r="GV3" s="3"/>
-      <c r="GW3" s="2"/>
-      <c r="GX3" s="2"/>
       <c r="GY3" s="1"/>
       <c r="GZ3" s="1"/>
       <c r="HA3" s="1"/>
       <c r="HB3" s="1"/>
       <c r="HC3" s="1"/>
       <c r="HD3" s="3"/>
-      <c r="HE3" s="2"/>
-      <c r="HF3" s="2"/>
       <c r="HG3" s="1"/>
       <c r="HH3" s="1"/>
       <c r="HI3" s="1"/>
       <c r="HJ3" s="1"/>
       <c r="HK3" s="1"/>
       <c r="HL3" s="3"/>
-      <c r="HM3" s="2"/>
-      <c r="HN3" s="2"/>
       <c r="HO3" s="1"/>
       <c r="HP3" s="1"/>
       <c r="HQ3" s="1"/>
       <c r="HR3" s="1"/>
       <c r="HS3" s="1"/>
       <c r="HT3" s="3"/>
-      <c r="HU3" s="2"/>
-      <c r="HV3" s="2"/>
       <c r="HW3" s="1"/>
       <c r="HX3" s="1"/>
       <c r="HY3" s="1"/>
       <c r="HZ3" s="1"/>
       <c r="IA3" s="1"/>
       <c r="IB3" s="3"/>
-      <c r="IC3" s="2"/>
-      <c r="ID3" s="2"/>
       <c r="IE3" s="1"/>
       <c r="IF3" s="1"/>
       <c r="IG3" s="1"/>
       <c r="IH3" s="1"/>
       <c r="II3" s="1"/>
       <c r="IJ3" s="3"/>
-      <c r="IK3" s="2"/>
-      <c r="IL3" s="2"/>
       <c r="IM3" s="1"/>
       <c r="IN3" s="1"/>
       <c r="IO3" s="1"/>
       <c r="IP3" s="1"/>
       <c r="IQ3" s="1"/>
       <c r="IR3" s="3"/>
-      <c r="IS3" s="2"/>
-      <c r="IT3" s="2"/>
-    </row>
-    <row r="4" spans="1:254" ht="29.25" customHeight="1">
-      <c r="A4" s="72" t="s">
+    </row>
+    <row r="4" spans="1:252" ht="29.25" customHeight="1">
+      <c r="A4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="74" t="s">
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="73" t="s">
+      <c r="J4" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:254" ht="19.5" customHeight="1">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:254" ht="25.5" customHeight="1">
-      <c r="A6" s="72" t="s">
+      <c r="K4" s="46"/>
+    </row>
+    <row r="5" spans="1:252" ht="19.5" customHeight="1">
+      <c r="A5" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="10">
+        <v>956439834</v>
+      </c>
+      <c r="J5" s="82">
+        <v>45042</v>
+      </c>
+      <c r="K5" s="48"/>
+    </row>
+    <row r="6" spans="1:252" ht="25.5" customHeight="1">
+      <c r="A6" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="74" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="75"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:254" ht="25.5" customHeight="1">
-      <c r="A7" s="77" t="s">
+      <c r="K6" s="46"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:252" ht="25.5" customHeight="1">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="G7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="35"/>
-      <c r="M7" s="12"/>
-    </row>
-    <row r="8" spans="1:254" ht="40.5" customHeight="1">
+      <c r="I7" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="82">
+        <v>45056</v>
+      </c>
+      <c r="K7" s="48"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:252" ht="40.5" customHeight="1">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="N8" s="12"/>
-    </row>
-    <row r="9" spans="1:254" ht="48.75" customHeight="1">
-      <c r="A9" s="72" t="s">
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="75"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:252" ht="48.75" customHeight="1">
+      <c r="A9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74" t="s">
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="73" t="s">
+      <c r="F9" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73" t="s">
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="75"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-    </row>
-    <row r="10" spans="1:254">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-    </row>
-    <row r="11" spans="1:254">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="70"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:254">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:254">
-      <c r="A13" s="57"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="70"/>
-    </row>
-    <row r="14" spans="1:254">
-      <c r="A14" s="60"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="71"/>
-    </row>
-    <row r="15" spans="1:254" ht="32.25" customHeight="1">
-      <c r="A15" s="39" t="s">
+      <c r="K9" s="46"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:252">
+      <c r="A10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="42"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:252">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:252">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:252">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:252">
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="44"/>
+    </row>
+    <row r="15" spans="1:252" ht="32.25" customHeight="1">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
-    </row>
-    <row r="16" spans="1:254" ht="32.25" customHeight="1">
-      <c r="A16" s="78" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:252" ht="32.25" customHeight="1">
+      <c r="A16" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79" t="s">
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="80" t="s">
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="81" t="s">
+      <c r="H16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81" t="s">
+      <c r="I16" s="24"/>
+      <c r="J16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="82"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="25"/>
+      <c r="A17" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="84">
+        <v>45032</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="25"/>
+      <c r="A18" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="84">
+        <v>45042</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="25"/>
+      <c r="A19" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="84">
+        <v>45048</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="27"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="25"/>
+      <c r="A20" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="84">
+        <v>45051</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="27"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="24"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="72"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="85" t="s">
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85" t="s">
+      <c r="G23" s="66"/>
+      <c r="H23" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="85"/>
-      <c r="J23" s="86" t="s">
+      <c r="I23" s="66"/>
+      <c r="J23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K23" s="87"/>
-    </row>
-    <row r="24" spans="1:11" ht="22.5" customHeight="1">
-      <c r="A24" s="19"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="38"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" spans="1:11" ht="35.4" customHeight="1">
+      <c r="A24" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="73"/>
+      <c r="H24" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="69"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="74"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="88" t="s">
+      <c r="A25" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="89"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="85" t="s">
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85" t="s">
+      <c r="G25" s="66"/>
+      <c r="H25" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="85"/>
-      <c r="J25" s="86" t="s">
+      <c r="I25" s="66"/>
+      <c r="J25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K25" s="87"/>
-    </row>
-    <row r="26" spans="1:11" ht="22.5" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="37"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" spans="1:11" ht="36" customHeight="1">
+      <c r="A26" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="91"/>
+      <c r="H26" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="68"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="K29" s="13"/>
+      <c r="K29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="A10:D14"/>
-    <mergeCell ref="E10:E14"/>
-    <mergeCell ref="F10:I14"/>
-    <mergeCell ref="J10:K14"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B1:I2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="F23:G23"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="A21:C21"/>
@@ -2367,6 +2465,38 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="A22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B1:I2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A10:D14"/>
+    <mergeCell ref="E10:E14"/>
+    <mergeCell ref="F10:I14"/>
+    <mergeCell ref="J10:K14"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="D18:F18"/>
@@ -2374,30 +2504,11 @@
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="H18:I18"/>
     <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:H6"/>
     <mergeCell ref="H20:I20"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="126" scale="91" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>